<commit_message>
update SailGP Standaings post Saint Tropez
</commit_message>
<xml_diff>
--- a/sailgp/season5-standings.xlsx
+++ b/sailgp/season5-standings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\tidbyt-data\tidbyt-data\sailgp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3725FD-23F3-42F4-9A14-FBDFE72B32A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE420842-ADC4-422F-91DB-92548A21061C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{E2D6DEE4-A194-47E1-9326-7C7ACA5A1011}"/>
   </bookViews>
@@ -455,12 +455,12 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C13"/>
+      <selection activeCell="A3" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -468,75 +468,75 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>61</v>
-      </c>
-      <c r="B2">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
         <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>61</v>
-      </c>
-      <c r="B3">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>58</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>56</v>
-      </c>
-      <c r="B5">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>47</v>
-      </c>
-      <c r="B6">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
         <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>44</v>
-      </c>
-      <c r="B7">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
         <v>6</v>
       </c>
     </row>
@@ -544,70 +544,70 @@
       <c r="A8">
         <v>30</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
         <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>22</v>
-      </c>
-      <c r="B9">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
         <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>20</v>
-      </c>
-      <c r="B10">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
         <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>-8</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C13">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B13">
     <sortCondition descending="1" ref="A2:A13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>